<commit_message>
Separated out Vernier Caliper instructions from instrumentation lab
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2020fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2020fall.xlsx
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="210">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -941,6 +941,12 @@
   </si>
   <si>
     <t>by Jerry, 2020</t>
+  </si>
+  <si>
+    <t>Vernier Caliper</t>
+  </si>
+  <si>
+    <t>Separated from Instrumentation 2020</t>
   </si>
 </sst>
 </file>
@@ -1827,28 +1833,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDFFCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -2179,10 +2164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD122"/>
+  <dimension ref="A1:AD123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q92" sqref="Q92"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3177,16 +3162,16 @@
         <v>0</v>
       </c>
       <c r="X23" s="6">
-        <f t="shared" ref="X23:X31" si="1">SUMIF(U$2:U$81,"&gt;=" &amp; W23,C$2:C$81)</f>
-        <v>329</v>
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W23,C$2:C$82)</f>
+        <v>330</v>
       </c>
       <c r="Y23" s="6">
-        <f t="shared" ref="Y23:Y31" si="2">SUMIF(U$2:U$81,"&gt;=" &amp; W23,D$2:D$81)</f>
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W23,D$2:D$82)</f>
         <v>11</v>
       </c>
       <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="3">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
-        <v>29.574999999999999</v>
+        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+        <v>29.64</v>
       </c>
       <c r="AA23" s="31"/>
       <c r="AB23" s="31"/>
@@ -3251,16 +3236,16 @@
         <v>0.5</v>
       </c>
       <c r="X24" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W24,C$2:C$82)</f>
+        <v>242</v>
+      </c>
+      <c r="Y24" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W24,D$2:D$82)</f>
+        <v>10</v>
+      </c>
+      <c r="Z24" s="8">
         <f t="shared" si="1"/>
-        <v>245</v>
-      </c>
-      <c r="Y24" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z24" s="8">
-        <f t="shared" si="3"/>
-        <v>23.725000000000001</v>
+        <v>23.53</v>
       </c>
       <c r="AA24" s="31"/>
       <c r="AB24" s="31"/>
@@ -3307,15 +3292,15 @@
         <v>1</v>
       </c>
       <c r="X25" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W25,C$2:C$82)</f>
+        <v>236</v>
+      </c>
+      <c r="Y25" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W25,D$2:D$82)</f>
+        <v>10</v>
+      </c>
+      <c r="Z25" s="8">
         <f t="shared" si="1"/>
-        <v>236</v>
-      </c>
-      <c r="Y25" s="6">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="Z25" s="8">
-        <f t="shared" si="3"/>
         <v>23.14</v>
       </c>
       <c r="AA25" s="31"/>
@@ -3371,16 +3356,16 @@
         <v>1.5</v>
       </c>
       <c r="X26" s="29">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,C$2:C$82)</f>
+        <v>124</v>
+      </c>
+      <c r="Y26" s="29">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,D$2:D$82)</f>
+        <v>2</v>
+      </c>
+      <c r="Z26" s="8">
         <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="Y26" s="29">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="Z26" s="8">
-        <f t="shared" si="3"/>
-        <v>12.545000000000002</v>
+        <v>12.739999999999998</v>
       </c>
       <c r="AA26" s="31"/>
       <c r="AB26" s="31"/>
@@ -3447,15 +3432,15 @@
         <v>2</v>
       </c>
       <c r="X27" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,C$2:C$82)</f>
+        <v>113</v>
+      </c>
+      <c r="Y27" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,D$2:D$82)</f>
+        <v>2</v>
+      </c>
+      <c r="Z27" s="8">
         <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="Y27" s="6">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="Z27" s="8">
-        <f t="shared" si="3"/>
         <v>12.025</v>
       </c>
     </row>
@@ -3507,15 +3492,15 @@
         <v>2.5</v>
       </c>
       <c r="X28" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,C$2:C$82)</f>
+        <v>6</v>
+      </c>
+      <c r="Y28" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,D$2:D$82)</f>
+        <v>1</v>
+      </c>
+      <c r="Z28" s="8">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="Y28" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Z28" s="8">
-        <f t="shared" si="3"/>
         <v>4.68</v>
       </c>
     </row>
@@ -3549,15 +3534,15 @@
         <v>3</v>
       </c>
       <c r="X29" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,C$2:C$82)</f>
+        <v>6</v>
+      </c>
+      <c r="Y29" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,D$2:D$82)</f>
+        <v>1</v>
+      </c>
+      <c r="Z29" s="8">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="Y29" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Z29" s="8">
-        <f t="shared" si="3"/>
         <v>4.68</v>
       </c>
     </row>
@@ -3609,15 +3594,15 @@
         <v>3.5</v>
       </c>
       <c r="X30" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,C$2:C$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,D$2:D$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y30" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="8">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -3650,15 +3635,15 @@
         <v>4</v>
       </c>
       <c r="X31" s="45">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,C$2:C$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="45">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,D$2:D$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y31" s="45">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="9">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
@@ -5312,10 +5297,12 @@
       </c>
       <c r="R68" s="34"/>
       <c r="S68" s="34"/>
-      <c r="T68" s="34"/>
+      <c r="T68" s="34">
+        <v>1</v>
+      </c>
       <c r="U68" s="74">
-        <f t="shared" ref="U68:U80" si="4">SUM(Q68:T68)</f>
-        <v>0.5</v>
+        <f t="shared" ref="U68:U81" si="2">SUM(Q68:T68)</f>
+        <v>1.5</v>
       </c>
       <c r="V68" s="14"/>
       <c r="W68" s="3"/>
@@ -5350,7 +5337,7 @@
       <c r="S69" s="34"/>
       <c r="T69" s="34"/>
       <c r="U69" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V69" s="14"/>
@@ -5386,7 +5373,7 @@
       <c r="S70" s="34"/>
       <c r="T70" s="34"/>
       <c r="U70" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V70" s="14"/>
@@ -5424,7 +5411,7 @@
       <c r="S71" s="34"/>
       <c r="T71" s="34"/>
       <c r="U71" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V71" s="14"/>
@@ -5455,7 +5442,7 @@
       </c>
       <c r="T72" s="32"/>
       <c r="U72" s="83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V72" s="14"/>
@@ -5504,7 +5491,7 @@
       <c r="S73" s="33"/>
       <c r="T73" s="33"/>
       <c r="U73" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V73" s="14"/>
@@ -5551,7 +5538,7 @@
       <c r="S74" s="34"/>
       <c r="T74" s="34"/>
       <c r="U74" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V74" s="14"/>
@@ -5579,7 +5566,7 @@
       </c>
       <c r="T75" s="32"/>
       <c r="U75" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V75" s="14"/>
@@ -5628,7 +5615,7 @@
       <c r="S76" s="34"/>
       <c r="T76" s="32"/>
       <c r="U76" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V76" s="14"/>
@@ -5651,7 +5638,7 @@
       </c>
       <c r="T77" s="32"/>
       <c r="U77" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V77" s="14"/>
@@ -5696,7 +5683,7 @@
       </c>
       <c r="T78" s="32"/>
       <c r="U78" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V78" s="14"/>
@@ -5743,7 +5730,7 @@
       <c r="S79" s="34"/>
       <c r="T79" s="32"/>
       <c r="U79" s="74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V79" s="14"/>
@@ -5756,266 +5743,268 @@
       <c r="AC79"/>
       <c r="AD79"/>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="B80" s="23" t="s">
+    <row r="80" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="10"/>
+      <c r="B80" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C80" s="13">
+        <v>1</v>
+      </c>
+      <c r="D80" s="13">
+        <v>0</v>
+      </c>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="J80" s="34"/>
+      <c r="K80" s="34"/>
+      <c r="L80" s="34"/>
+      <c r="M80" s="34"/>
+      <c r="N80" s="34"/>
+      <c r="O80" s="34"/>
+      <c r="P80" s="34"/>
+      <c r="Q80" s="34">
+        <v>1</v>
+      </c>
+      <c r="R80" s="34"/>
+      <c r="S80" s="34"/>
+      <c r="T80" s="32"/>
+      <c r="U80" s="74">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V80" s="14"/>
+      <c r="W80" s="3"/>
+      <c r="X80" s="31"/>
+      <c r="Y80" s="31"/>
+      <c r="Z80" s="31"/>
+      <c r="AA80" s="31"/>
+      <c r="AB80" s="31"/>
+      <c r="AC80" s="31"/>
+      <c r="AD80" s="31"/>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B81" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="26">
+      <c r="C81" s="26">
         <v>4</v>
       </c>
-      <c r="D80" s="26">
+      <c r="D81" s="26">
         <v>0</v>
       </c>
-      <c r="E80" s="26"/>
-      <c r="F80" s="26"/>
-      <c r="G80" s="26"/>
-      <c r="H80" s="26"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="35"/>
-      <c r="K80" s="35"/>
-      <c r="L80" s="35"/>
-      <c r="M80" s="35">
-        <v>1</v>
-      </c>
-      <c r="N80" s="35">
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="27"/>
+      <c r="J81" s="35"/>
+      <c r="K81" s="35"/>
+      <c r="L81" s="35"/>
+      <c r="M81" s="35">
+        <v>1</v>
+      </c>
+      <c r="N81" s="35">
         <v>0</v>
       </c>
-      <c r="O80" s="35">
-        <v>1</v>
-      </c>
-      <c r="P80" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q80" s="35">
-        <v>1</v>
-      </c>
-      <c r="R80" s="35"/>
-      <c r="S80" s="35"/>
-      <c r="T80" s="35"/>
-      <c r="U80" s="83">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V80" s="14"/>
-    </row>
-    <row r="81" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="11"/>
+      <c r="O81" s="35">
+        <v>1</v>
+      </c>
+      <c r="P81" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="35">
+        <v>0</v>
+      </c>
+      <c r="R81" s="35"/>
+      <c r="S81" s="35"/>
+      <c r="T81" s="35"/>
+      <c r="U81" s="83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="V81" s="14"/>
-      <c r="Y81" s="31"/>
-    </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I82" s="61" t="s">
+    </row>
+    <row r="82" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="11"/>
+      <c r="V82" s="14"/>
+      <c r="Y82" s="31"/>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I83" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="J82" s="80"/>
-      <c r="K82" s="62"/>
-      <c r="L82" s="62"/>
-      <c r="M82" s="62"/>
-      <c r="N82" s="62"/>
-      <c r="O82" s="62">
-        <f t="array" ref="O82">SUM($C2:$C80*(O2:O80&gt;=0.9)*($U2:$U80&gt;=$W$12))</f>
-        <v>184</v>
-      </c>
-      <c r="P82" s="62">
-        <f t="array" ref="P82">SUM($C2:$C80*(P2:P80&gt;=0.9)*($U2:$U80&gt;=$W$12))</f>
-        <v>195</v>
-      </c>
-      <c r="Q82" s="62">
-        <f t="array" ref="Q82">SUM($C2:$C80*(Q2:Q80&gt;=0.9)*($U2:$U80&gt;=$W$12))</f>
-        <v>200</v>
-      </c>
-      <c r="R82" s="62">
-        <f t="array" ref="R82">SUM($C2:$C80*(R2:R80&gt;=0.9)*($U2:$U80&gt;=$W$12))</f>
+      <c r="J83" s="80"/>
+      <c r="K83" s="62"/>
+      <c r="L83" s="62"/>
+      <c r="M83" s="62"/>
+      <c r="N83" s="62"/>
+      <c r="O83" s="62"/>
+      <c r="P83" s="62"/>
+      <c r="Q83" s="62">
+        <f t="array" ref="Q83">SUM($C2:$C81*(Q2:Q81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
+        <v>197</v>
+      </c>
+      <c r="R83" s="62">
+        <f t="array" ref="R83">SUM($C2:$C81*(R2:R81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
         <v>126</v>
       </c>
-      <c r="S82" s="62"/>
-      <c r="T82" s="63"/>
-      <c r="V82" s="14"/>
-      <c r="AA82" s="6"/>
-      <c r="AB82" s="6"/>
-      <c r="AC82" s="6"/>
-      <c r="AD82" s="6"/>
-    </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="I83" s="64" t="s">
+      <c r="S83" s="62"/>
+      <c r="T83" s="63"/>
+      <c r="V83" s="14"/>
+      <c r="AA83" s="6"/>
+      <c r="AB83" s="6"/>
+      <c r="AC83" s="6"/>
+      <c r="AD83" s="6"/>
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I84" s="64" t="s">
         <v>100</v>
-      </c>
-      <c r="J83" s="81"/>
-      <c r="K83" s="65"/>
-      <c r="L83" s="65"/>
-      <c r="M83" s="65"/>
-      <c r="N83" s="65"/>
-      <c r="O83" s="65">
-        <f t="array" ref="O83">SUM($C2:$C80*O2:O80*($U2:$U80&gt;=$W$12))</f>
-        <v>202</v>
-      </c>
-      <c r="P83" s="65">
-        <f t="array" ref="P83">SUM($C2:$C80*P2:P80*($U2:$U80&gt;=$W$12))</f>
-        <v>199.5</v>
-      </c>
-      <c r="Q83" s="65">
-        <f t="array" ref="Q83">SUM($C2:$C80*Q2:Q80*($U2:$U80&gt;=$W$12))</f>
-        <v>204</v>
-      </c>
-      <c r="R83" s="65">
-        <f t="array" ref="R83">SUM($C2:$C80*R2:R80*($U2:$U80&gt;=$W$12))</f>
-        <v>126</v>
-      </c>
-      <c r="S83" s="65"/>
-      <c r="T83" s="66"/>
-      <c r="V83" s="14"/>
-    </row>
-    <row r="84" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="10"/>
-      <c r="B84" s="22"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="64" t="s">
-        <v>99</v>
       </c>
       <c r="J84" s="81"/>
       <c r="K84" s="65"/>
       <c r="L84" s="65"/>
       <c r="M84" s="65"/>
       <c r="N84" s="65"/>
-      <c r="O84" s="65">
-        <f t="array" ref="O84">SUM($C$2:$C$80*(O$2:O$80&gt;=0.1)*($U$2:$U$80&gt;=$W$12))</f>
-        <v>209</v>
-      </c>
-      <c r="P84" s="65">
-        <f t="array" ref="P84">SUM($C$2:$C$80*(P$2:P$80&gt;=0.1)*($U$2:$U$80&gt;=$W$12))</f>
-        <v>204</v>
-      </c>
+      <c r="O84" s="65"/>
+      <c r="P84" s="65"/>
       <c r="Q84" s="65">
-        <f t="array" ref="Q84">SUM($C$2:$C$80*(Q$2:Q$80&gt;=0.1)*($U$2:$U$80&gt;=$W$12))</f>
-        <v>208</v>
+        <f t="array" ref="Q84">SUM($C2:$C81*Q2:Q81*($U2:$U81&gt;=$W$12))</f>
+        <v>202.5</v>
       </c>
       <c r="R84" s="65">
-        <f t="array" ref="R84">SUM($C$2:$C$80*(R$2:R$80&gt;=0.1)*($U$2:$U$80&gt;=$W$12))</f>
+        <f t="array" ref="R84">SUM($C2:$C81*R2:R81*($U2:$U81&gt;=$W$12))</f>
         <v>126</v>
       </c>
       <c r="S84" s="65"/>
       <c r="T84" s="66"/>
-      <c r="U84" s="3"/>
       <c r="V84" s="14"/>
-      <c r="W84" s="3"/>
-      <c r="X84"/>
-      <c r="Y84"/>
-      <c r="Z84"/>
-      <c r="AA84"/>
-      <c r="AB84"/>
-      <c r="AC84"/>
-      <c r="AD84"/>
-    </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="10"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
       <c r="I85" s="64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J85" s="81"/>
       <c r="K85" s="65"/>
       <c r="L85" s="65"/>
       <c r="M85" s="65"/>
       <c r="N85" s="65"/>
-      <c r="O85" s="65">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>236</v>
-      </c>
-      <c r="P85" s="65">
-        <f>LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>236</v>
-      </c>
+      <c r="O85" s="65"/>
+      <c r="P85" s="65"/>
       <c r="Q85" s="65">
-        <f t="shared" ref="Q85:R85" si="5">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>236</v>
+        <f t="array" ref="Q85">SUM($C$2:$C$81*(Q$2:Q$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
+        <v>208</v>
       </c>
       <c r="R85" s="65">
-        <f t="shared" si="5"/>
-        <v>236</v>
+        <f t="array" ref="R85">SUM($C$2:$C$81*(R$2:R$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
+        <v>126</v>
       </c>
       <c r="S85" s="65"/>
       <c r="T85" s="66"/>
+      <c r="U85" s="3"/>
       <c r="V85" s="14"/>
-      <c r="AA85" s="6"/>
-      <c r="AB85" s="6"/>
-      <c r="AC85" s="6"/>
-      <c r="AD85" s="6"/>
+      <c r="W85" s="3"/>
+      <c r="X85"/>
+      <c r="Y85"/>
+      <c r="Z85"/>
+      <c r="AA85"/>
+      <c r="AB85"/>
+      <c r="AC85"/>
+      <c r="AD85"/>
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I86" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="J86" s="81"/>
+      <c r="K86" s="65"/>
+      <c r="L86" s="65"/>
+      <c r="M86" s="65"/>
+      <c r="N86" s="65"/>
+      <c r="O86" s="65"/>
+      <c r="P86" s="65"/>
+      <c r="Q86" s="65">
+        <f t="shared" ref="Q86:R86" si="3">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>236</v>
+      </c>
+      <c r="R86" s="65">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="S86" s="65"/>
+      <c r="T86" s="66"/>
+      <c r="V86" s="14"/>
+      <c r="AA86" s="6"/>
+      <c r="AB86" s="6"/>
+      <c r="AC86" s="6"/>
+      <c r="AD86" s="6"/>
+    </row>
+    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I87" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="J86" s="81"/>
-      <c r="K86" s="67"/>
-      <c r="L86" s="67"/>
-      <c r="M86" s="67"/>
-      <c r="N86" s="67"/>
-      <c r="O86" s="67">
-        <f>O83/O85</f>
-        <v>0.85593220338983056</v>
-      </c>
-      <c r="P86" s="67">
-        <f>P83/P85</f>
-        <v>0.84533898305084743</v>
-      </c>
-      <c r="Q86" s="67">
-        <f t="shared" ref="Q86:R86" si="6">Q83/Q85</f>
-        <v>0.86440677966101698</v>
-      </c>
-      <c r="R86" s="67">
-        <f t="shared" si="6"/>
+      <c r="J87" s="81"/>
+      <c r="K87" s="67"/>
+      <c r="L87" s="67"/>
+      <c r="M87" s="67"/>
+      <c r="N87" s="67"/>
+      <c r="O87" s="67"/>
+      <c r="P87" s="67"/>
+      <c r="Q87" s="67">
+        <f t="shared" ref="Q87:R87" si="4">Q84/Q86</f>
+        <v>0.85805084745762716</v>
+      </c>
+      <c r="R87" s="67">
+        <f t="shared" si="4"/>
         <v>0.53389830508474578</v>
       </c>
-      <c r="S86" s="67"/>
-      <c r="T86" s="68"/>
-      <c r="V86" s="14"/>
-    </row>
-    <row r="87" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C87" s="31"/>
-      <c r="I87" s="69" t="s">
+      <c r="S87" s="67"/>
+      <c r="T87" s="68"/>
+      <c r="V87" s="14"/>
+    </row>
+    <row r="88" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="31"/>
+      <c r="I88" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="J87" s="82"/>
-      <c r="K87" s="70"/>
-      <c r="L87" s="70"/>
-      <c r="M87" s="70"/>
-      <c r="N87" s="70"/>
-      <c r="O87" s="70">
-        <f>O85-O83</f>
-        <v>34</v>
-      </c>
-      <c r="P87" s="70">
-        <f>P85-P83</f>
-        <v>36.5</v>
-      </c>
-      <c r="Q87" s="70">
-        <f t="shared" ref="Q87:R87" si="7">Q85-Q83</f>
-        <v>32</v>
-      </c>
-      <c r="R87" s="70">
-        <f t="shared" si="7"/>
+      <c r="J88" s="82"/>
+      <c r="K88" s="70"/>
+      <c r="L88" s="70"/>
+      <c r="M88" s="70"/>
+      <c r="N88" s="70"/>
+      <c r="O88" s="70"/>
+      <c r="P88" s="70"/>
+      <c r="Q88" s="70">
+        <f t="shared" ref="Q88:R88" si="5">Q86-Q84</f>
+        <v>33.5</v>
+      </c>
+      <c r="R88" s="70">
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
-      <c r="S87" s="70"/>
-      <c r="T87" s="71"/>
-      <c r="V87" s="14"/>
-      <c r="AA87" s="6"/>
-      <c r="AB87" s="6"/>
-      <c r="AC87" s="6"/>
-      <c r="AD87" s="6"/>
-    </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="C88" s="31"/>
+      <c r="S88" s="70"/>
+      <c r="T88" s="71"/>
       <c r="V88" s="14"/>
+      <c r="AA88" s="6"/>
+      <c r="AB88" s="6"/>
+      <c r="AC88" s="6"/>
+      <c r="AD88" s="6"/>
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C89" s="31"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
       <c r="V89" s="14"/>
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.3">
@@ -6026,6 +6015,7 @@
       <c r="V90" s="14"/>
     </row>
     <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C91" s="31"/>
       <c r="I91" s="13"/>
       <c r="J91" s="13"/>
       <c r="K91" s="13"/>
@@ -6036,18 +6026,19 @@
       <c r="J92" s="13"/>
       <c r="K92" s="13"/>
       <c r="V92" s="14"/>
-      <c r="Z92" s="31"/>
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I93" s="13"/>
       <c r="J93" s="13"/>
       <c r="K93" s="13"/>
       <c r="V93" s="14"/>
+      <c r="Z93" s="31"/>
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I94" s="13"/>
       <c r="J94" s="13"/>
       <c r="K94" s="13"/>
+      <c r="V94" s="14"/>
     </row>
     <row r="95" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I95" s="13"/>
@@ -6059,71 +6050,76 @@
       <c r="J96" s="13"/>
       <c r="K96" s="13"/>
     </row>
-    <row r="97" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="10"/>
-      <c r="B97" s="22"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="19"/>
-      <c r="J97" s="34"/>
-      <c r="K97" s="34"/>
-      <c r="L97" s="34"/>
-      <c r="M97" s="34"/>
-      <c r="N97" s="34"/>
-      <c r="O97" s="34"/>
-      <c r="P97" s="34"/>
-      <c r="Q97" s="34"/>
-      <c r="R97" s="34"/>
-      <c r="S97" s="34"/>
-      <c r="T97" s="2"/>
-      <c r="U97" s="3"/>
-      <c r="V97" s="3"/>
-      <c r="W97" s="3"/>
-      <c r="X97"/>
-      <c r="Y97"/>
-      <c r="Z97"/>
-      <c r="AA97"/>
-      <c r="AB97"/>
-      <c r="AC97"/>
-      <c r="AD97"/>
-    </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA100" s="6"/>
-      <c r="AB100" s="6"/>
-      <c r="AC100" s="6"/>
-      <c r="AD100" s="6"/>
-    </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA104" s="6"/>
-      <c r="AB104" s="6"/>
-      <c r="AC104" s="6"/>
-      <c r="AD104" s="6"/>
-    </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA109" s="6"/>
-      <c r="AB109" s="6"/>
-      <c r="AC109" s="6"/>
-      <c r="AD109" s="6"/>
-    </row>
-    <row r="122" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA122" s="31"/>
-      <c r="AB122" s="31"/>
-      <c r="AC122" s="31"/>
-      <c r="AD122" s="31"/>
+    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+      <c r="K97" s="13"/>
+    </row>
+    <row r="98" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="10"/>
+      <c r="B98" s="22"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="19"/>
+      <c r="J98" s="34"/>
+      <c r="K98" s="34"/>
+      <c r="L98" s="34"/>
+      <c r="M98" s="34"/>
+      <c r="N98" s="34"/>
+      <c r="O98" s="34"/>
+      <c r="P98" s="34"/>
+      <c r="Q98" s="34"/>
+      <c r="R98" s="34"/>
+      <c r="S98" s="34"/>
+      <c r="T98" s="2"/>
+      <c r="U98" s="3"/>
+      <c r="V98" s="3"/>
+      <c r="W98" s="3"/>
+      <c r="X98"/>
+      <c r="Y98"/>
+      <c r="Z98"/>
+      <c r="AA98"/>
+      <c r="AB98"/>
+      <c r="AC98"/>
+      <c r="AD98"/>
+    </row>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA101" s="6"/>
+      <c r="AB101" s="6"/>
+      <c r="AC101" s="6"/>
+      <c r="AD101" s="6"/>
+    </row>
+    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA105" s="6"/>
+      <c r="AB105" s="6"/>
+      <c r="AC105" s="6"/>
+      <c r="AD105" s="6"/>
+    </row>
+    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA110" s="6"/>
+      <c r="AB110" s="6"/>
+      <c r="AC110" s="6"/>
+      <c r="AD110" s="6"/>
+    </row>
+    <row r="123" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA123" s="31"/>
+      <c r="AB123" s="31"/>
+      <c r="AC123" s="31"/>
+      <c r="AD123" s="31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U80">
-    <cfRule type="expression" dxfId="5" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B2:U81">
+    <cfRule type="expression" dxfId="2" priority="43" stopIfTrue="1">
       <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="44" stopIfTrue="1">
       <formula>$U2&gt;=$W$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="45">
+    <cfRule type="expression" dxfId="0" priority="45">
       <formula>$U2&gt;=($W$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>